<commit_message>
ASMD Load n Store.
</commit_message>
<xml_diff>
--- a/ArquiProjecto/Phase2/ControlStateDiagram_M.xlsx
+++ b/ArquiProjecto/Phase2/ControlStateDiagram_M.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2234" uniqueCount="200">
   <si>
     <t>BRANCH</t>
   </si>
@@ -1117,7 +1117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1222,16 +1222,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1516,8 +1519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L86" sqref="L86"/>
+    <sheetView tabSelected="1" topLeftCell="Z68" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL78" sqref="AL78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1552,30 +1555,30 @@
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
       <c r="P2" s="13"/>
-      <c r="Q2" s="42" t="s">
+      <c r="Q2" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
       <c r="T2" s="13"/>
       <c r="U2" s="7" t="s">
         <v>69</v>
@@ -1592,21 +1595,21 @@
         <v>72</v>
       </c>
       <c r="AB2" s="13"/>
-      <c r="AC2" s="43" t="s">
+      <c r="AC2" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AD2" s="43"/>
+      <c r="AD2" s="44"/>
       <c r="AE2" s="23"/>
       <c r="AF2" s="18" t="s">
         <v>74</v>
       </c>
       <c r="AG2" s="13"/>
-      <c r="AH2" s="43" t="s">
+      <c r="AH2" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="AI2" s="43"/>
-      <c r="AJ2" s="43"/>
-      <c r="AK2" s="43"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
@@ -1979,13 +1982,13 @@
       <c r="AK6" s="39">
         <v>0</v>
       </c>
-      <c r="AL6" s="44" t="s">
+      <c r="AL6" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="AM6" s="44"/>
-      <c r="AN6" s="44"/>
-      <c r="AO6" s="44"/>
-      <c r="AP6" s="44"/>
+      <c r="AM6" s="46"/>
+      <c r="AN6" s="46"/>
+      <c r="AO6" s="46"/>
+      <c r="AP6" s="46"/>
       <c r="AQ6" s="27"/>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.55000000000000004">
@@ -2301,30 +2304,30 @@
       <c r="A12" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
-      <c r="I12" s="43" t="s">
+      <c r="I12" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
       <c r="P12" s="13"/>
-      <c r="Q12" s="42" t="s">
+      <c r="Q12" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
       <c r="T12" s="13"/>
       <c r="U12" s="7" t="s">
         <v>69</v>
@@ -2341,21 +2344,21 @@
         <v>72</v>
       </c>
       <c r="AB12" s="13"/>
-      <c r="AC12" s="43" t="s">
+      <c r="AC12" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AD12" s="43"/>
+      <c r="AD12" s="44"/>
       <c r="AE12" s="23"/>
       <c r="AF12" s="18" t="s">
         <v>74</v>
       </c>
       <c r="AG12" s="13"/>
-      <c r="AH12" s="43" t="s">
+      <c r="AH12" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="AI12" s="43"/>
-      <c r="AJ12" s="43"/>
-      <c r="AK12" s="43"/>
+      <c r="AI12" s="44"/>
+      <c r="AJ12" s="44"/>
+      <c r="AK12" s="44"/>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
@@ -5469,40 +5472,40 @@
       <c r="A47" s="16"/>
       <c r="B47" s="13"/>
       <c r="C47" s="28"/>
-      <c r="D47" s="44" t="s">
+      <c r="D47" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="44"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
-      <c r="K47" s="44"/>
-      <c r="L47" s="44"/>
-      <c r="M47" s="44"/>
-      <c r="N47" s="44"/>
-      <c r="O47" s="44"/>
-      <c r="P47" s="44"/>
-      <c r="Q47" s="44"/>
-      <c r="R47" s="44"/>
-      <c r="S47" s="44"/>
-      <c r="T47" s="44"/>
-      <c r="U47" s="44"/>
-      <c r="V47" s="44"/>
-      <c r="W47" s="44"/>
-      <c r="X47" s="44"/>
-      <c r="Y47" s="44"/>
-      <c r="Z47" s="44"/>
-      <c r="AA47" s="44"/>
-      <c r="AB47" s="44"/>
-      <c r="AC47" s="44"/>
-      <c r="AD47" s="44"/>
-      <c r="AE47" s="44"/>
-      <c r="AF47" s="44"/>
-      <c r="AG47" s="44"/>
-      <c r="AH47" s="44"/>
-      <c r="AI47" s="44"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
+      <c r="M47" s="46"/>
+      <c r="N47" s="46"/>
+      <c r="O47" s="46"/>
+      <c r="P47" s="46"/>
+      <c r="Q47" s="46"/>
+      <c r="R47" s="46"/>
+      <c r="S47" s="46"/>
+      <c r="T47" s="46"/>
+      <c r="U47" s="46"/>
+      <c r="V47" s="46"/>
+      <c r="W47" s="46"/>
+      <c r="X47" s="46"/>
+      <c r="Y47" s="46"/>
+      <c r="Z47" s="46"/>
+      <c r="AA47" s="46"/>
+      <c r="AB47" s="46"/>
+      <c r="AC47" s="46"/>
+      <c r="AD47" s="46"/>
+      <c r="AE47" s="46"/>
+      <c r="AF47" s="46"/>
+      <c r="AG47" s="46"/>
+      <c r="AH47" s="46"/>
+      <c r="AI47" s="46"/>
       <c r="AJ47" s="13"/>
       <c r="AK47" s="13"/>
     </row>
@@ -5551,30 +5554,30 @@
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
       <c r="F49" s="20"/>
       <c r="G49" s="20"/>
       <c r="H49" s="20"/>
-      <c r="I49" s="43" t="s">
+      <c r="I49" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43"/>
-      <c r="M49" s="43"/>
-      <c r="N49" s="43"/>
-      <c r="O49" s="43"/>
+      <c r="J49" s="44"/>
+      <c r="K49" s="44"/>
+      <c r="L49" s="44"/>
+      <c r="M49" s="44"/>
+      <c r="N49" s="44"/>
+      <c r="O49" s="44"/>
       <c r="P49" s="13"/>
-      <c r="Q49" s="42" t="s">
+      <c r="Q49" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="R49" s="42"/>
-      <c r="S49" s="42"/>
+      <c r="R49" s="43"/>
+      <c r="S49" s="43"/>
       <c r="T49" s="13"/>
       <c r="U49" s="7" t="s">
         <v>69</v>
@@ -5591,21 +5594,21 @@
         <v>72</v>
       </c>
       <c r="AB49" s="13"/>
-      <c r="AC49" s="43" t="s">
+      <c r="AC49" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AD49" s="43"/>
+      <c r="AD49" s="44"/>
       <c r="AE49" s="23"/>
       <c r="AF49" s="18" t="s">
         <v>74</v>
       </c>
       <c r="AG49" s="13"/>
-      <c r="AH49" s="43" t="s">
+      <c r="AH49" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="AI49" s="43"/>
-      <c r="AJ49" s="43"/>
-      <c r="AK49" s="43"/>
+      <c r="AI49" s="44"/>
+      <c r="AJ49" s="44"/>
+      <c r="AK49" s="44"/>
     </row>
     <row r="50" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2" t="s">
@@ -7898,54 +7901,54 @@
         <v>27</v>
       </c>
       <c r="O77" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="P77" s="40"/>
+        <v>28</v>
+      </c>
+      <c r="P77" s="42"/>
       <c r="Q77" s="39" t="s">
         <v>78</v>
       </c>
       <c r="R77" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="S77" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="T77" s="40"/>
+      <c r="S77" s="39">
+        <v>1</v>
+      </c>
+      <c r="T77" s="42"/>
       <c r="U77" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="V77" s="40"/>
+        <v>29</v>
+      </c>
+      <c r="V77" s="42"/>
       <c r="W77" s="39">
         <v>1</v>
       </c>
-      <c r="X77" s="40"/>
+      <c r="X77" s="42"/>
       <c r="Y77" s="39">
         <v>1</v>
       </c>
-      <c r="Z77" s="40"/>
+      <c r="Z77" s="42"/>
       <c r="AA77" s="39">
         <v>1</v>
       </c>
-      <c r="AB77" s="40"/>
+      <c r="AB77" s="42"/>
       <c r="AC77" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD77" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="AE77" s="40"/>
+      <c r="AE77" s="42"/>
       <c r="AF77" s="39">
-        <v>1</v>
-      </c>
-      <c r="AG77" s="40"/>
-      <c r="AH77" s="39" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="AG77" s="42"/>
+      <c r="AH77" s="41" t="s">
+        <v>148</v>
       </c>
       <c r="AI77" s="39" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="AJ77" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK77" s="39">
         <v>1</v>
@@ -7993,7 +7996,7 @@
       <c r="O78" s="39">
         <v>10</v>
       </c>
-      <c r="P78" s="40"/>
+      <c r="P78" s="42"/>
       <c r="Q78" s="41" t="s">
         <v>151</v>
       </c>
@@ -8003,34 +8006,34 @@
       <c r="S78" s="39">
         <v>1</v>
       </c>
-      <c r="T78" s="40"/>
+      <c r="T78" s="42"/>
       <c r="U78" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="V78" s="40"/>
+      <c r="V78" s="42"/>
       <c r="W78" s="39">
         <v>1</v>
       </c>
-      <c r="X78" s="40"/>
+      <c r="X78" s="42"/>
       <c r="Y78" s="39">
         <v>1</v>
       </c>
-      <c r="Z78" s="40"/>
+      <c r="Z78" s="42"/>
       <c r="AA78" s="39">
         <v>1</v>
       </c>
-      <c r="AB78" s="40"/>
+      <c r="AB78" s="42"/>
       <c r="AC78" s="39">
         <v>1</v>
       </c>
       <c r="AD78" s="39">
         <v>1</v>
       </c>
-      <c r="AE78" s="40"/>
+      <c r="AE78" s="42"/>
       <c r="AF78" s="39">
         <v>0</v>
       </c>
-      <c r="AG78" s="40"/>
+      <c r="AG78" s="42"/>
       <c r="AH78" s="39" t="s">
         <v>28</v>
       </c>
@@ -8128,30 +8131,30 @@
       <c r="A81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B81" s="42" t="s">
+      <c r="B81" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C81" s="42"/>
-      <c r="D81" s="42"/>
-      <c r="E81" s="42"/>
+      <c r="C81" s="43"/>
+      <c r="D81" s="43"/>
+      <c r="E81" s="43"/>
       <c r="F81" s="20"/>
       <c r="G81" s="20"/>
       <c r="H81" s="20"/>
-      <c r="I81" s="43" t="s">
+      <c r="I81" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="J81" s="43"/>
-      <c r="K81" s="43"/>
-      <c r="L81" s="43"/>
-      <c r="M81" s="43"/>
-      <c r="N81" s="43"/>
-      <c r="O81" s="43"/>
+      <c r="J81" s="44"/>
+      <c r="K81" s="44"/>
+      <c r="L81" s="44"/>
+      <c r="M81" s="44"/>
+      <c r="N81" s="44"/>
+      <c r="O81" s="44"/>
       <c r="P81" s="13"/>
-      <c r="Q81" s="42" t="s">
+      <c r="Q81" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="R81" s="42"/>
-      <c r="S81" s="42"/>
+      <c r="R81" s="43"/>
+      <c r="S81" s="43"/>
       <c r="T81" s="13"/>
       <c r="U81" s="7" t="s">
         <v>69</v>
@@ -8168,21 +8171,21 @@
         <v>72</v>
       </c>
       <c r="AB81" s="13"/>
-      <c r="AC81" s="43" t="s">
+      <c r="AC81" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AD81" s="43"/>
+      <c r="AD81" s="44"/>
       <c r="AE81" s="23"/>
       <c r="AF81" s="18" t="s">
         <v>74</v>
       </c>
       <c r="AG81" s="13"/>
-      <c r="AH81" s="43" t="s">
+      <c r="AH81" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="AI81" s="43"/>
-      <c r="AJ81" s="43"/>
-      <c r="AK81" s="43"/>
+      <c r="AI81" s="44"/>
+      <c r="AJ81" s="44"/>
+      <c r="AK81" s="44"/>
     </row>
     <row r="82" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="2" t="s">
@@ -10477,7 +10480,7 @@
       <c r="O109" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="P109" s="40"/>
+      <c r="P109" s="42"/>
       <c r="Q109" s="39" t="s">
         <v>78</v>
       </c>
@@ -10487,34 +10490,34 @@
       <c r="S109" s="39">
         <v>1</v>
       </c>
-      <c r="T109" s="40"/>
+      <c r="T109" s="42"/>
       <c r="U109" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="V109" s="40"/>
+      <c r="V109" s="42"/>
       <c r="W109" s="39">
         <v>1</v>
       </c>
-      <c r="X109" s="40"/>
+      <c r="X109" s="42"/>
       <c r="Y109" s="39">
         <v>1</v>
       </c>
-      <c r="Z109" s="40"/>
+      <c r="Z109" s="42"/>
       <c r="AA109" s="39">
         <v>1</v>
       </c>
-      <c r="AB109" s="40"/>
+      <c r="AB109" s="42"/>
       <c r="AC109" s="39">
         <v>0</v>
       </c>
       <c r="AD109" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="AE109" s="40"/>
+      <c r="AE109" s="42"/>
       <c r="AF109" s="39">
         <v>0</v>
       </c>
-      <c r="AG109" s="40"/>
+      <c r="AG109" s="42"/>
       <c r="AH109" s="41" t="s">
         <v>148</v>
       </c>
@@ -10570,7 +10573,7 @@
       <c r="O110" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="P110" s="40"/>
+      <c r="P110" s="42"/>
       <c r="Q110" s="39" t="s">
         <v>78</v>
       </c>
@@ -10580,34 +10583,34 @@
       <c r="S110" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="T110" s="40"/>
+      <c r="T110" s="42"/>
       <c r="U110" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="V110" s="40"/>
+      <c r="V110" s="42"/>
       <c r="W110" s="39">
         <v>1</v>
       </c>
-      <c r="X110" s="40"/>
+      <c r="X110" s="42"/>
       <c r="Y110" s="39">
         <v>1</v>
       </c>
-      <c r="Z110" s="40"/>
+      <c r="Z110" s="42"/>
       <c r="AA110" s="39">
         <v>1</v>
       </c>
-      <c r="AB110" s="40"/>
+      <c r="AB110" s="42"/>
       <c r="AC110" s="39">
         <v>1</v>
       </c>
       <c r="AD110" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="AE110" s="40"/>
+      <c r="AE110" s="42"/>
       <c r="AF110" s="39">
         <v>0</v>
       </c>
-      <c r="AG110" s="40"/>
+      <c r="AG110" s="42"/>
       <c r="AH110" s="41" t="s">
         <v>148</v>
       </c>
@@ -10705,30 +10708,30 @@
       <c r="A113" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B113" s="42" t="s">
+      <c r="B113" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C113" s="42"/>
-      <c r="D113" s="42"/>
-      <c r="E113" s="42"/>
+      <c r="C113" s="43"/>
+      <c r="D113" s="43"/>
+      <c r="E113" s="43"/>
       <c r="F113" s="20"/>
       <c r="G113" s="20"/>
       <c r="H113" s="20"/>
-      <c r="I113" s="43" t="s">
+      <c r="I113" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="J113" s="43"/>
-      <c r="K113" s="43"/>
-      <c r="L113" s="43"/>
-      <c r="M113" s="43"/>
-      <c r="N113" s="43"/>
-      <c r="O113" s="43"/>
+      <c r="J113" s="44"/>
+      <c r="K113" s="44"/>
+      <c r="L113" s="44"/>
+      <c r="M113" s="44"/>
+      <c r="N113" s="44"/>
+      <c r="O113" s="44"/>
       <c r="P113" s="13"/>
-      <c r="Q113" s="42" t="s">
+      <c r="Q113" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="R113" s="42"/>
-      <c r="S113" s="42"/>
+      <c r="R113" s="43"/>
+      <c r="S113" s="43"/>
       <c r="T113" s="13"/>
       <c r="U113" s="7" t="s">
         <v>69</v>
@@ -10745,21 +10748,21 @@
         <v>72</v>
       </c>
       <c r="AB113" s="13"/>
-      <c r="AC113" s="43" t="s">
+      <c r="AC113" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AD113" s="43"/>
+      <c r="AD113" s="44"/>
       <c r="AE113" s="23"/>
       <c r="AF113" s="18" t="s">
         <v>74</v>
       </c>
       <c r="AG113" s="13"/>
-      <c r="AH113" s="43" t="s">
+      <c r="AH113" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="AI113" s="43"/>
-      <c r="AJ113" s="43"/>
-      <c r="AK113" s="43"/>
+      <c r="AI113" s="44"/>
+      <c r="AJ113" s="44"/>
+      <c r="AK113" s="44"/>
     </row>
     <row r="114" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="2" t="s">
@@ -11887,75 +11890,75 @@
         <v>0</v>
       </c>
       <c r="H127" s="21"/>
-      <c r="I127" s="9">
-        <v>1</v>
-      </c>
-      <c r="J127" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K127" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L127" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M127" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="N127" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="O127" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="P127" s="13"/>
-      <c r="Q127" s="9" t="s">
+      <c r="I127" s="39">
+        <v>1</v>
+      </c>
+      <c r="J127" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="K127" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="L127" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="M127" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="N127" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="O127" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="P127" s="42"/>
+      <c r="Q127" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="R127" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="S127" s="9">
-        <v>1</v>
-      </c>
-      <c r="T127" s="13"/>
-      <c r="U127" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="V127" s="13"/>
-      <c r="W127" s="9">
-        <v>1</v>
-      </c>
-      <c r="X127" s="13"/>
-      <c r="Y127" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z127" s="13"/>
-      <c r="AA127" s="9">
-        <v>1</v>
-      </c>
-      <c r="AB127" s="13"/>
-      <c r="AC127" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD127" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE127" s="13"/>
-      <c r="AF127" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG127" s="13"/>
-      <c r="AH127" s="17" t="s">
+      <c r="R127" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="S127" s="39">
+        <v>1</v>
+      </c>
+      <c r="T127" s="42"/>
+      <c r="U127" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="V127" s="42"/>
+      <c r="W127" s="39">
+        <v>1</v>
+      </c>
+      <c r="X127" s="42"/>
+      <c r="Y127" s="39">
+        <v>1</v>
+      </c>
+      <c r="Z127" s="42"/>
+      <c r="AA127" s="39">
+        <v>1</v>
+      </c>
+      <c r="AB127" s="42"/>
+      <c r="AC127" s="39">
+        <v>0</v>
+      </c>
+      <c r="AD127" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE127" s="42"/>
+      <c r="AF127" s="39">
+        <v>0</v>
+      </c>
+      <c r="AG127" s="42"/>
+      <c r="AH127" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="AI127" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ127" s="9">
-        <v>1</v>
-      </c>
-      <c r="AK127" s="9">
+      <c r="AI127" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ127" s="39">
+        <v>1</v>
+      </c>
+      <c r="AK127" s="39">
         <v>1</v>
       </c>
     </row>
@@ -12136,30 +12139,30 @@
       <c r="A131" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B131" s="42" t="s">
+      <c r="B131" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C131" s="42"/>
-      <c r="D131" s="42"/>
-      <c r="E131" s="42"/>
+      <c r="C131" s="43"/>
+      <c r="D131" s="43"/>
+      <c r="E131" s="43"/>
       <c r="F131" s="20"/>
       <c r="G131" s="20"/>
       <c r="H131" s="20"/>
-      <c r="I131" s="43" t="s">
+      <c r="I131" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="J131" s="43"/>
-      <c r="K131" s="43"/>
-      <c r="L131" s="43"/>
-      <c r="M131" s="43"/>
-      <c r="N131" s="43"/>
-      <c r="O131" s="43"/>
+      <c r="J131" s="44"/>
+      <c r="K131" s="44"/>
+      <c r="L131" s="44"/>
+      <c r="M131" s="44"/>
+      <c r="N131" s="44"/>
+      <c r="O131" s="44"/>
       <c r="P131" s="13"/>
-      <c r="Q131" s="42" t="s">
+      <c r="Q131" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="R131" s="42"/>
-      <c r="S131" s="42"/>
+      <c r="R131" s="43"/>
+      <c r="S131" s="43"/>
       <c r="T131" s="13"/>
       <c r="U131" s="7" t="s">
         <v>69</v>
@@ -12176,21 +12179,21 @@
         <v>72</v>
       </c>
       <c r="AB131" s="13"/>
-      <c r="AC131" s="43" t="s">
+      <c r="AC131" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AD131" s="43"/>
+      <c r="AD131" s="44"/>
       <c r="AE131" s="23"/>
       <c r="AF131" s="18" t="s">
         <v>74</v>
       </c>
       <c r="AG131" s="13"/>
-      <c r="AH131" s="43" t="s">
+      <c r="AH131" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="AI131" s="43"/>
-      <c r="AJ131" s="43"/>
-      <c r="AK131" s="43"/>
+      <c r="AI131" s="44"/>
+      <c r="AJ131" s="44"/>
+      <c r="AK131" s="44"/>
     </row>
     <row r="132" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="2" t="s">
@@ -13526,30 +13529,30 @@
       <c r="A148" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B148" s="42" t="s">
+      <c r="B148" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C148" s="42"/>
-      <c r="D148" s="42"/>
-      <c r="E148" s="42"/>
+      <c r="C148" s="43"/>
+      <c r="D148" s="43"/>
+      <c r="E148" s="43"/>
       <c r="F148" s="20"/>
       <c r="G148" s="20"/>
       <c r="H148" s="20"/>
-      <c r="I148" s="43" t="s">
+      <c r="I148" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="J148" s="43"/>
-      <c r="K148" s="43"/>
-      <c r="L148" s="43"/>
-      <c r="M148" s="43"/>
-      <c r="N148" s="43"/>
-      <c r="O148" s="43"/>
+      <c r="J148" s="44"/>
+      <c r="K148" s="44"/>
+      <c r="L148" s="44"/>
+      <c r="M148" s="44"/>
+      <c r="N148" s="44"/>
+      <c r="O148" s="44"/>
       <c r="P148" s="13"/>
-      <c r="Q148" s="42" t="s">
+      <c r="Q148" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="R148" s="42"/>
-      <c r="S148" s="42"/>
+      <c r="R148" s="43"/>
+      <c r="S148" s="43"/>
       <c r="T148" s="13"/>
       <c r="U148" s="7" t="s">
         <v>69</v>
@@ -13566,21 +13569,21 @@
         <v>72</v>
       </c>
       <c r="AB148" s="13"/>
-      <c r="AC148" s="43" t="s">
+      <c r="AC148" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AD148" s="43"/>
+      <c r="AD148" s="44"/>
       <c r="AE148" s="23"/>
       <c r="AF148" s="18" t="s">
         <v>74</v>
       </c>
       <c r="AG148" s="13"/>
-      <c r="AH148" s="43" t="s">
+      <c r="AH148" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="AI148" s="43"/>
-      <c r="AJ148" s="43"/>
-      <c r="AK148" s="43"/>
+      <c r="AI148" s="44"/>
+      <c r="AJ148" s="44"/>
+      <c r="AK148" s="44"/>
     </row>
     <row r="149" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="2" t="s">
@@ -13811,30 +13814,30 @@
       <c r="A152" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B152" s="42" t="s">
+      <c r="B152" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C152" s="42"/>
-      <c r="D152" s="42"/>
-      <c r="E152" s="42"/>
+      <c r="C152" s="43"/>
+      <c r="D152" s="43"/>
+      <c r="E152" s="43"/>
       <c r="F152" s="20"/>
       <c r="G152" s="20"/>
       <c r="H152" s="20"/>
-      <c r="I152" s="43" t="s">
+      <c r="I152" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="J152" s="43"/>
-      <c r="K152" s="43"/>
-      <c r="L152" s="43"/>
-      <c r="M152" s="43"/>
-      <c r="N152" s="43"/>
-      <c r="O152" s="43"/>
+      <c r="J152" s="44"/>
+      <c r="K152" s="44"/>
+      <c r="L152" s="44"/>
+      <c r="M152" s="44"/>
+      <c r="N152" s="44"/>
+      <c r="O152" s="44"/>
       <c r="P152" s="13"/>
-      <c r="Q152" s="42" t="s">
+      <c r="Q152" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="R152" s="42"/>
-      <c r="S152" s="42"/>
+      <c r="R152" s="43"/>
+      <c r="S152" s="43"/>
       <c r="T152" s="13"/>
       <c r="U152" s="7" t="s">
         <v>69</v>
@@ -13851,21 +13854,21 @@
         <v>72</v>
       </c>
       <c r="AB152" s="13"/>
-      <c r="AC152" s="43" t="s">
+      <c r="AC152" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AD152" s="43"/>
+      <c r="AD152" s="44"/>
       <c r="AE152" s="23"/>
       <c r="AF152" s="18" t="s">
         <v>74</v>
       </c>
       <c r="AG152" s="13"/>
-      <c r="AH152" s="43" t="s">
+      <c r="AH152" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="AI152" s="43"/>
-      <c r="AJ152" s="43"/>
-      <c r="AK152" s="43"/>
+      <c r="AI152" s="44"/>
+      <c r="AJ152" s="44"/>
+      <c r="AK152" s="44"/>
     </row>
     <row r="153" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="2" t="s">
@@ -14095,30 +14098,30 @@
       <c r="A156" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B156" s="42" t="s">
+      <c r="B156" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C156" s="42"/>
-      <c r="D156" s="42"/>
-      <c r="E156" s="42"/>
+      <c r="C156" s="43"/>
+      <c r="D156" s="43"/>
+      <c r="E156" s="43"/>
       <c r="F156" s="20"/>
       <c r="G156" s="20"/>
       <c r="H156" s="20"/>
-      <c r="I156" s="43" t="s">
+      <c r="I156" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="J156" s="43"/>
-      <c r="K156" s="43"/>
-      <c r="L156" s="43"/>
-      <c r="M156" s="43"/>
-      <c r="N156" s="43"/>
-      <c r="O156" s="43"/>
+      <c r="J156" s="44"/>
+      <c r="K156" s="44"/>
+      <c r="L156" s="44"/>
+      <c r="M156" s="44"/>
+      <c r="N156" s="44"/>
+      <c r="O156" s="44"/>
       <c r="P156" s="13"/>
-      <c r="Q156" s="42" t="s">
+      <c r="Q156" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="R156" s="42"/>
-      <c r="S156" s="42"/>
+      <c r="R156" s="43"/>
+      <c r="S156" s="43"/>
       <c r="T156" s="13"/>
       <c r="U156" s="7" t="s">
         <v>69</v>
@@ -14135,21 +14138,21 @@
         <v>72</v>
       </c>
       <c r="AB156" s="13"/>
-      <c r="AC156" s="43" t="s">
+      <c r="AC156" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AD156" s="43"/>
+      <c r="AD156" s="44"/>
       <c r="AE156" s="23"/>
       <c r="AF156" s="18" t="s">
         <v>74</v>
       </c>
       <c r="AG156" s="13"/>
-      <c r="AH156" s="43" t="s">
+      <c r="AH156" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="AI156" s="43"/>
-      <c r="AJ156" s="43"/>
-      <c r="AK156" s="43"/>
+      <c r="AI156" s="44"/>
+      <c r="AJ156" s="44"/>
+      <c r="AK156" s="44"/>
     </row>
     <row r="157" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="2" t="s">
@@ -14332,30 +14335,30 @@
       <c r="A160" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B160" s="42" t="s">
+      <c r="B160" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C160" s="42"/>
-      <c r="D160" s="42"/>
-      <c r="E160" s="42"/>
+      <c r="C160" s="43"/>
+      <c r="D160" s="43"/>
+      <c r="E160" s="43"/>
       <c r="F160" s="20"/>
       <c r="G160" s="20"/>
       <c r="H160" s="20"/>
-      <c r="I160" s="43" t="s">
+      <c r="I160" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="J160" s="43"/>
-      <c r="K160" s="43"/>
-      <c r="L160" s="43"/>
-      <c r="M160" s="43"/>
-      <c r="N160" s="43"/>
-      <c r="O160" s="43"/>
+      <c r="J160" s="44"/>
+      <c r="K160" s="44"/>
+      <c r="L160" s="44"/>
+      <c r="M160" s="44"/>
+      <c r="N160" s="44"/>
+      <c r="O160" s="44"/>
       <c r="P160" s="13"/>
-      <c r="Q160" s="42" t="s">
+      <c r="Q160" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="R160" s="42"/>
-      <c r="S160" s="42"/>
+      <c r="R160" s="43"/>
+      <c r="S160" s="43"/>
       <c r="T160" s="13"/>
       <c r="U160" s="7" t="s">
         <v>69</v>
@@ -14372,21 +14375,21 @@
         <v>72</v>
       </c>
       <c r="AB160" s="13"/>
-      <c r="AC160" s="43" t="s">
+      <c r="AC160" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AD160" s="43"/>
+      <c r="AD160" s="44"/>
       <c r="AE160" s="23"/>
       <c r="AF160" s="18" t="s">
         <v>74</v>
       </c>
       <c r="AG160" s="13"/>
-      <c r="AH160" s="43" t="s">
+      <c r="AH160" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="AI160" s="43"/>
-      <c r="AJ160" s="43"/>
-      <c r="AK160" s="43"/>
+      <c r="AI160" s="44"/>
+      <c r="AJ160" s="44"/>
+      <c r="AK160" s="44"/>
     </row>
     <row r="161" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="2" t="s">
@@ -14717,6 +14720,47 @@
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="B160:E160"/>
+    <mergeCell ref="AC160:AD160"/>
+    <mergeCell ref="AH160:AK160"/>
+    <mergeCell ref="I160:O160"/>
+    <mergeCell ref="Q160:S160"/>
+    <mergeCell ref="B156:E156"/>
+    <mergeCell ref="AC156:AD156"/>
+    <mergeCell ref="AH156:AK156"/>
+    <mergeCell ref="I156:O156"/>
+    <mergeCell ref="Q156:S156"/>
+    <mergeCell ref="AL6:AP6"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AH12:AK12"/>
+    <mergeCell ref="AH49:AK49"/>
+    <mergeCell ref="AI11:AK11"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="I49:O49"/>
+    <mergeCell ref="I12:O12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q49:S49"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="I11:N11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="Q152:S152"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="AH81:AK81"/>
+    <mergeCell ref="B113:E113"/>
+    <mergeCell ref="AH113:AK113"/>
+    <mergeCell ref="B131:E131"/>
+    <mergeCell ref="AH131:AK131"/>
+    <mergeCell ref="I81:O81"/>
+    <mergeCell ref="I113:O113"/>
+    <mergeCell ref="I131:O131"/>
+    <mergeCell ref="Q81:S81"/>
+    <mergeCell ref="Q113:S113"/>
+    <mergeCell ref="Q131:S131"/>
     <mergeCell ref="B148:E148"/>
     <mergeCell ref="B152:E152"/>
     <mergeCell ref="AC2:AD2"/>
@@ -14733,47 +14777,6 @@
     <mergeCell ref="I148:O148"/>
     <mergeCell ref="I152:O152"/>
     <mergeCell ref="Q148:S148"/>
-    <mergeCell ref="Q152:S152"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="AH81:AK81"/>
-    <mergeCell ref="B113:E113"/>
-    <mergeCell ref="AH113:AK113"/>
-    <mergeCell ref="B131:E131"/>
-    <mergeCell ref="AH131:AK131"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="I11:N11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="AL6:AP6"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AH12:AK12"/>
-    <mergeCell ref="AH49:AK49"/>
-    <mergeCell ref="AI11:AK11"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="I49:O49"/>
-    <mergeCell ref="B156:E156"/>
-    <mergeCell ref="AC156:AD156"/>
-    <mergeCell ref="AH156:AK156"/>
-    <mergeCell ref="I156:O156"/>
-    <mergeCell ref="Q156:S156"/>
-    <mergeCell ref="B160:E160"/>
-    <mergeCell ref="AC160:AD160"/>
-    <mergeCell ref="AH160:AK160"/>
-    <mergeCell ref="I160:O160"/>
-    <mergeCell ref="Q160:S160"/>
-    <mergeCell ref="I12:O12"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="I81:O81"/>
-    <mergeCell ref="I113:O113"/>
-    <mergeCell ref="I131:O131"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q49:S49"/>
-    <mergeCell ref="Q81:S81"/>
-    <mergeCell ref="Q113:S113"/>
-    <mergeCell ref="Q131:S131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>